<commit_message>
update new hero 112
</commit_message>
<xml_diff>
--- a/opm_hero_property/design/hero_design.xlsx
+++ b/opm_hero_property/design/hero_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="32600"/>
+    <workbookView windowWidth="21600"/>
   </bookViews>
   <sheets>
     <sheet name="卡牌设定" sheetId="1" r:id="rId1"/>
@@ -543,9 +543,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -602,6 +602,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -609,7 +616,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -617,13 +624,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -638,10 +638,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -653,40 +662,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -699,24 +677,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,7 +716,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -752,7 +752,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,169 +932,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,9 +966,50 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -988,36 +1029,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1032,162 +1043,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1195,7 +1195,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1255,6 +1255,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1584,11 +1587,11 @@
   <dimension ref="A1:X127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M87" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W113" sqref="W113"/>
+      <selection pane="bottomRight" activeCell="W95" sqref="W95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4"/>
@@ -9242,25 +9245,25 @@
         <v>1</v>
       </c>
       <c r="Q102" s="2">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="R102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U102" s="2">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="V102" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W102" s="2">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="X102" s="14">
         <f t="shared" si="2"/>
@@ -9314,28 +9317,28 @@
         <v>0</v>
       </c>
       <c r="P103" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q103" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R103" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S103" s="2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V103" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W103" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X103" s="14">
         <f t="shared" si="2"/>
@@ -10017,50 +10020,122 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="113" spans="9:9">
-      <c r="I113" s="23"/>
+    <row r="113" spans="1:24">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113" s="13">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1.015</v>
+      </c>
+      <c r="E113" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F113" s="2">
+        <v>1</v>
+      </c>
+      <c r="G113" s="2">
+        <v>30003</v>
+      </c>
+      <c r="H113" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="I113" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="J113" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K113" s="14">
+        <v>0</v>
+      </c>
+      <c r="L113" s="14">
+        <v>0</v>
+      </c>
+      <c r="M113" s="14">
+        <v>0</v>
+      </c>
+      <c r="N113" s="14">
+        <v>0.0025</v>
+      </c>
+      <c r="O113" s="14">
+        <v>0</v>
+      </c>
+      <c r="P113" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q113" s="2">
+        <v>-4</v>
+      </c>
+      <c r="R113" s="14">
+        <v>0</v>
+      </c>
+      <c r="S113" s="14">
+        <v>3</v>
+      </c>
+      <c r="T113" s="14">
+        <v>0</v>
+      </c>
+      <c r="U113" s="14">
+        <v>0</v>
+      </c>
+      <c r="V113" s="14">
+        <v>0</v>
+      </c>
+      <c r="W113" s="14">
+        <v>3</v>
+      </c>
+      <c r="X113" s="14">
+        <f>SUM(R113:T113)/2+SUM(U113:W113)</f>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="114" spans="9:9">
-      <c r="I114" s="23"/>
+      <c r="I114" s="24"/>
     </row>
     <row r="115" spans="9:9">
-      <c r="I115" s="23"/>
+      <c r="I115" s="24"/>
     </row>
     <row r="116" spans="9:9">
-      <c r="I116" s="23"/>
+      <c r="I116" s="24"/>
     </row>
     <row r="117" spans="9:9">
-      <c r="I117" s="23"/>
+      <c r="I117" s="24"/>
     </row>
     <row r="118" spans="9:9">
-      <c r="I118" s="23"/>
+      <c r="I118" s="24"/>
     </row>
     <row r="119" spans="9:9">
-      <c r="I119" s="23"/>
+      <c r="I119" s="24"/>
     </row>
     <row r="120" spans="9:9">
-      <c r="I120" s="23"/>
+      <c r="I120" s="24"/>
     </row>
     <row r="121" spans="9:9">
-      <c r="I121" s="23"/>
+      <c r="I121" s="24"/>
     </row>
     <row r="122" spans="9:9">
-      <c r="I122" s="23"/>
+      <c r="I122" s="24"/>
     </row>
     <row r="123" spans="9:9">
-      <c r="I123" s="23"/>
+      <c r="I123" s="24"/>
     </row>
     <row r="124" spans="9:9">
-      <c r="I124" s="23"/>
+      <c r="I124" s="24"/>
     </row>
     <row r="125" spans="9:9">
-      <c r="I125" s="23"/>
+      <c r="I125" s="24"/>
     </row>
     <row r="126" spans="9:9">
-      <c r="I126" s="23"/>
+      <c r="I126" s="24"/>
     </row>
     <row r="127" spans="9:9">
-      <c r="I127" s="23"/>
+      <c r="I127" s="24"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P$1:P$1048576">
@@ -10072,7 +10147,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{76849758-6825-40e4-90c3-a4821c6481e7}</x14:id>
+          <x14:id>{bd0d9cea-25b5-4db4-85de-2fb553737190}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10096,7 +10171,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{76849758-6825-40e4-90c3-a4821c6481e7}">
+          <x14:cfRule type="dataBar" id="{bd0d9cea-25b5-4db4-85de-2fb553737190}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>